<commit_message>
Add first boxscore (live-ish updates) support
</commit_message>
<xml_diff>
--- a/src/main/resources/team_colors.xlsx
+++ b/src/main/resources/team_colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tclarke\git\football-prediction\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BD3C2C92-6EF7-46AA-B713-42C9B2A0FAEF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E40DD983-3DF8-4AF7-A24A-6D925C9FC4DA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="750">
   <si>
     <t>Air Force</t>
   </si>
@@ -2237,9 +2237,6 @@
   </si>
   <si>
     <t>#354ca1</t>
-  </si>
-  <si>
-    <t>#cc0035</t>
   </si>
   <si>
     <t>#d00000</t>
@@ -2632,8 +2629,8 @@
   </sheetPr>
   <dimension ref="A1:E433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="C272" sqref="C272"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="G334" sqref="G334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4504,7 +4501,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -5060,10 +5057,10 @@
         <v>367</v>
       </c>
       <c r="B202" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="C202" s="1" t="s">
         <v>743</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>744</v>
       </c>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -5190,7 +5187,7 @@
         <v>386</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
@@ -5454,10 +5451,10 @@
         <v>423</v>
       </c>
       <c r="B236" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="C236" s="1" t="s">
         <v>740</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>741</v>
       </c>
       <c r="D236" s="1"/>
       <c r="E236" s="1"/>
@@ -5795,7 +5792,7 @@
         <v>469</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C265" s="1" t="s">
         <v>34</v>
@@ -5885,7 +5882,7 @@
         <v>169</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D272" s="1"/>
       <c r="E272" s="1"/>
@@ -6017,7 +6014,7 @@
         <v>495</v>
       </c>
       <c r="B283" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C283" s="1" t="s">
         <v>496</v>
@@ -6283,7 +6280,7 @@
         <v>534</v>
       </c>
       <c r="B305" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C305" s="1" t="s">
         <v>11</v>
@@ -6660,9 +6657,11 @@
         <v>738</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="D335" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="D335" s="1" t="s">
+        <v>738</v>
+      </c>
       <c r="E335" s="1"/>
     </row>
     <row r="336" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -7729,7 +7728,7 @@
         <v>719</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C427" s="1" t="s">
         <v>11</v>

</xml_diff>